<commit_message>
SWV et LWV fonctionnel , petit fix dans les signaux internes du datapath
</commit_message>
<xml_diff>
--- a/TestUnitaires.xlsx
+++ b/TestUnitaires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\PCArchitecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F5CF10-2D97-4A31-9E87-7A07969AA860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ABBA6A-E9F4-4409-A318-92542FCE0D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2066EFEB-9789-482C-AA6E-A8247BD797D8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>TEST UNITAIRE</t>
   </si>
@@ -81,7 +81,57 @@
     <t>0x2 dans ,les 4 registres</t>
   </si>
   <si>
-    <t>a</t>
+    <t xml:space="preserve">X"20100024", X"3c011001", X"C0280000", X"2002000a", X"0000000c", </t>
+  </si>
+  <si>
+    <t>Load  vectorielle a 0x10010000</t>
+  </si>
+  <si>
+    <t>Load de 0x1001000 jusqua 0x1001000c dans $t0 jusqua $t3 (reg 8 a 11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequence de donne utiliser pour les tests </t>
+  </si>
+  <si>
+    <t>X"12345678",
+X"87654321",
+X"bad0face",
+X"00000001",
+X"00000002",
+X"00000003",
+X"00000004",
+X"00000005",
+X"00000006",
+X"5555cccc",</t>
+  </si>
+  <si>
+    <t>12345678 dans $t0,  87654321 dans  $t1,  bad0face dans $t2, 1 dans $t3</t>
+  </si>
+  <si>
+    <t>12345678 dans $t0, 87654321 dans $t1, bad0face dans $t2, 1 dans $t3</t>
+  </si>
+  <si>
+    <t>X"20100024",
+X"3c011001",
+X"20080001",
+X"20090002",
+X"200a0003",
+X"200b0004",
+X"C4280000",
+X"2002000a",
+X"0000000c",</t>
+  </si>
+  <si>
+    <t>intialise 1,2,3,4 dans $t0 a $t3, ensuite save $t0 -$t3 dans la memoire (a partir de 0x10010000 qui est le debut des donnees)</t>
+  </si>
+  <si>
+    <t>retrouver 1,2,3,4 dans 0x10010000, 0x10010004 , 0x10010008, 0x1001000c resespectivement</t>
+  </si>
+  <si>
+    <t>on voit bien lupdate des valeurs dans la mémoire</t>
+  </si>
+  <si>
+    <t>save de 4 registres intialisés avec des valeurs aléatoire</t>
   </si>
 </sst>
 </file>
@@ -525,17 +575,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45E1DBD-2F4E-4269-8CAD-137E567F286D}">
-  <dimension ref="A3:T32"/>
+  <dimension ref="A3:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="28.42578125" customWidth="1"/>
+    <col min="18" max="18" width="24.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="20" max="20" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -543,11 +604,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="7" spans="1:20" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>1</v>
@@ -598,7 +654,7 @@
       </c>
       <c r="T9" s="5"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -620,14 +676,24 @@
       <c r="I10" s="8"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="2"/>
+      <c r="L10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="7"/>
+      <c r="O10" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
+      <c r="Q10" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="R10" s="7"/>
-      <c r="S10" s="8"/>
+      <c r="S10" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="T10" s="8"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -918,15 +984,25 @@
       </c>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="2"/>
+    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
+      <c r="H23" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="I23" s="8"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
@@ -1137,6 +1213,16 @@
       <c r="R32" s="7"/>
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="176">

</xml_diff>

<commit_message>
Ajout des formats d'instructions movnv et movzv
</commit_message>
<xml_diff>
--- a/TestUnitaires.xlsx
+++ b/TestUnitaires.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\PCArchitecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boldu\Documents\S4\APP4\Problématique\PCArchitecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C9016-ED96-4314-A71A-D1D1F3CC3918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BB8E26-2CB7-4AB9-9121-3AD04238FCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2066EFEB-9789-482C-AA6E-A8247BD797D8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="101">
   <si>
     <t>TEST UNITAIRE</t>
   </si>
@@ -197,12 +197,6 @@
   </si>
   <si>
     <t xml:space="preserve">immediate </t>
-  </si>
-  <si>
-    <t>MOVV</t>
-  </si>
-  <si>
-    <t>MOVZ</t>
   </si>
   <si>
     <t>adresse in mem</t>
@@ -374,6 +368,30 @@
   </si>
   <si>
     <t>SLTV sur des registres consecutif</t>
+  </si>
+  <si>
+    <t>registre operande binaire</t>
+  </si>
+  <si>
+    <t>registre operande</t>
+  </si>
+  <si>
+    <t>MOVNV  $s0, $t0, $t4</t>
+  </si>
+  <si>
+    <t>CD0C8000 - 110011 01000 01100 10000 00000 000000</t>
+  </si>
+  <si>
+    <t>CD0C8000 - 110110 01000 01100 10000 00000 000000</t>
+  </si>
+  <si>
+    <t>MOVNV  $s0, $t0, $s4</t>
+  </si>
+  <si>
+    <t>si $t0 - $t3 != 0, $s4-$s7 =  $s0-$s3</t>
+  </si>
+  <si>
+    <t>si $t0 - $t3 = 0, $t4-$t7 =  $s0-$s3</t>
   </si>
 </sst>
 </file>
@@ -527,10 +545,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -539,13 +564,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45E1DBD-2F4E-4269-8CAD-137E567F286D}">
   <dimension ref="A2:AG61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,23 +925,23 @@
     </row>
     <row r="4" spans="1:33" ht="28.5" x14ac:dyDescent="0.45">
       <c r="W4" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="AA5" s="18" t="s">
+      <c r="AA5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
       <c r="AD5" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AF5" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
@@ -963,24 +981,24 @@
         <v>110000</v>
       </c>
       <c r="Y7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA7" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="Z7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA7" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
       <c r="AD7" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AE7" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AF7" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,67 +1009,67 @@
         <v>110001</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA8" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
+        <v>49</v>
+      </c>
+      <c r="AA8" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
       <c r="AD8" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE8" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF8" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="AE8" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF8" s="14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21" t="s">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="21"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21" t="s">
+      <c r="N9" s="20"/>
+      <c r="O9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21" t="s">
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21" t="s">
+      <c r="R9" s="20"/>
+      <c r="S9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="T9" s="21"/>
+      <c r="T9" s="20"/>
       <c r="W9" s="4" t="s">
         <v>1</v>
       </c>
@@ -1059,13 +1077,13 @@
         <v>110010</v>
       </c>
       <c r="Y9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA9" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA9" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="AB9" s="4">
         <v>0</v>
@@ -1074,16 +1092,16 @@
         <v>100</v>
       </c>
       <c r="AD9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE9" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="AE9" s="15" t="s">
-        <v>78</v>
-      </c>
       <c r="AF9" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG9" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="AG9" s="15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="30" x14ac:dyDescent="0.25">
@@ -1091,9 +1109,9 @@
         <v>10</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="16"/>
+        <v>91</v>
+      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="17" t="s">
         <v>11</v>
       </c>
@@ -1102,19 +1120,19 @@
         <v>12</v>
       </c>
       <c r="G10" s="17"/>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="20"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="16"/>
+      <c r="N10" s="19"/>
       <c r="O10" s="17" t="s">
         <v>16</v>
       </c>
@@ -1123,10 +1141,10 @@
         <v>18</v>
       </c>
       <c r="R10" s="17"/>
-      <c r="S10" s="20" t="s">
+      <c r="S10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="T10" s="20"/>
+      <c r="T10" s="18"/>
       <c r="W10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1134,30 +1152,30 @@
         <v>110100</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Z10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA10" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
       <c r="AD10" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AE10" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF10" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="AF10" s="14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
@@ -1167,8 +1185,8 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
@@ -1182,13 +1200,13 @@
         <v>110101</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AA11" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB11" s="4">
         <v>0</v>
@@ -1197,19 +1215,19 @@
         <v>111</v>
       </c>
       <c r="AD11" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AE11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF11" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="AF11" s="14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
@@ -1219,8 +1237,8 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
@@ -1228,27 +1246,43 @@
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
       <c r="V12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="X12" s="4">
         <v>110011</v>
       </c>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="13"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Y12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF12" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -1258,8 +1292,8 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
@@ -1267,27 +1301,43 @@
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
       <c r="V13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="X13" s="4">
         <v>110110</v>
       </c>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="13"/>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
+      <c r="Y13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF13" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -1297,8 +1347,8 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="6"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
@@ -1318,8 +1368,8 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
@@ -1329,8 +1379,8 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="6"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
@@ -1340,8 +1390,8 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -1351,8 +1401,8 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="17"/>
@@ -1362,8 +1412,8 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -1373,8 +1423,8 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
@@ -1384,8 +1434,8 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -1395,8 +1445,8 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="17"/>
@@ -1406,8 +1456,8 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -1417,8 +1467,8 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
@@ -1426,7 +1476,7 @@
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
     </row>
-    <row r="20" spans="1:23" ht="52.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1451,8 +1501,8 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
-      <c r="W20" s="22" t="s">
-        <v>84</v>
+      <c r="W20" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -1477,52 +1527,52 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="W21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21" t="s">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21" t="s">
+      <c r="G22" s="20"/>
+      <c r="H22" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="21"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M22" s="21" t="s">
+      <c r="M22" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21" t="s">
+      <c r="N22" s="20"/>
+      <c r="O22" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21" t="s">
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21" t="s">
+      <c r="R22" s="20"/>
+      <c r="S22" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="T22" s="21"/>
+      <c r="T22" s="20"/>
       <c r="W22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -1532,7 +1582,7 @@
       <c r="B23" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="17" t="s">
         <v>21</v>
       </c>
@@ -1541,10 +1591,10 @@
         <v>22</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="18"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="5" t="s">
@@ -1553,7 +1603,7 @@
       <c r="M23" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="16"/>
+      <c r="N23" s="19"/>
       <c r="O23" s="17" t="s">
         <v>27</v>
       </c>
@@ -1562,18 +1612,18 @@
         <v>28</v>
       </c>
       <c r="R23" s="17"/>
-      <c r="S23" s="20" t="s">
+      <c r="S23" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="T23" s="20"/>
+      <c r="T23" s="18"/>
       <c r="W23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -1583,8 +1633,8 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17"/>
@@ -1594,8 +1644,8 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -1605,8 +1655,8 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="17"/>
@@ -1616,8 +1666,8 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
@@ -1627,8 +1677,8 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
@@ -1638,8 +1688,8 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -1649,8 +1699,8 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="6"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="17"/>
@@ -1660,8 +1710,8 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
@@ -1671,8 +1721,8 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="6"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
       <c r="Q28" s="17"/>
@@ -1682,8 +1732,8 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
@@ -1693,8 +1743,8 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="17"/>
@@ -1704,8 +1754,8 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
@@ -1715,8 +1765,8 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="6"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="17"/>
@@ -1726,8 +1776,8 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
@@ -1737,8 +1787,8 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="6"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="17"/>
@@ -1748,8 +1798,8 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
@@ -1759,8 +1809,8 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="6"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="17"/>
@@ -1816,84 +1866,84 @@
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21" t="s">
+      <c r="E36" s="20"/>
+      <c r="F36" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21" t="s">
+      <c r="G36" s="20"/>
+      <c r="H36" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I36" s="21"/>
+      <c r="I36" s="20"/>
       <c r="L36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M36" s="21" t="s">
+      <c r="M36" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21" t="s">
+      <c r="N36" s="20"/>
+      <c r="O36" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21" t="s">
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="R36" s="21"/>
-      <c r="S36" s="21" t="s">
+      <c r="R36" s="20"/>
+      <c r="S36" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="T36" s="21"/>
+      <c r="T36" s="20"/>
     </row>
     <row r="37" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G37" s="17"/>
-      <c r="H37" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="I37" s="20"/>
+      <c r="H37" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="18"/>
       <c r="L37" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M37" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="N37" s="19"/>
+      <c r="O37" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="N37" s="16"/>
-      <c r="O37" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="P37" s="17"/>
       <c r="Q37" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R37" s="17"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
@@ -1901,8 +1951,8 @@
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="L38" s="6"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
       <c r="O38" s="17"/>
       <c r="P38" s="17"/>
       <c r="Q38" s="17"/>
@@ -1912,8 +1962,8 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
@@ -1921,8 +1971,8 @@
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
       <c r="L39" s="6"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
       <c r="O39" s="17"/>
       <c r="P39" s="17"/>
       <c r="Q39" s="17"/>
@@ -1932,8 +1982,8 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
@@ -1941,8 +1991,8 @@
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
       <c r="L40" s="6"/>
-      <c r="M40" s="16"/>
-      <c r="N40" s="16"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
       <c r="O40" s="17"/>
       <c r="P40" s="17"/>
       <c r="Q40" s="17"/>
@@ -1952,8 +2002,8 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
@@ -1961,8 +2011,8 @@
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
       <c r="O41" s="17"/>
       <c r="P41" s="17"/>
       <c r="Q41" s="17"/>
@@ -1972,8 +2022,8 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
@@ -1981,8 +2031,8 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
       <c r="O42" s="17"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="17"/>
@@ -1992,8 +2042,8 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
@@ -2001,8 +2051,8 @@
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="L43" s="6"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
       <c r="O43" s="17"/>
       <c r="P43" s="17"/>
       <c r="Q43" s="17"/>
@@ -2012,8 +2062,8 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
@@ -2021,8 +2071,8 @@
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
       <c r="L44" s="6"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
       <c r="Q44" s="17"/>
@@ -2032,8 +2082,8 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
@@ -2041,8 +2091,8 @@
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
       <c r="L45" s="6"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
       <c r="Q45" s="17"/>
@@ -2052,8 +2102,8 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
@@ -2061,8 +2111,8 @@
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
       <c r="L46" s="6"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="16"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
       <c r="O46" s="17"/>
       <c r="P46" s="17"/>
       <c r="Q46" s="17"/>
@@ -2098,31 +2148,31 @@
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21" t="s">
+      <c r="C51" s="20"/>
+      <c r="D51" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21" t="s">
+      <c r="E51" s="20"/>
+      <c r="F51" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21" t="s">
+      <c r="G51" s="20"/>
+      <c r="H51" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I51" s="21"/>
+      <c r="I51" s="20"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="16"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="17" t="s">
         <v>34</v>
       </c>
@@ -2131,15 +2181,15 @@
         <v>35</v>
       </c>
       <c r="G52" s="17"/>
-      <c r="H52" s="20" t="s">
+      <c r="H52" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I52" s="20"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
@@ -2149,8 +2199,8 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
@@ -2160,8 +2210,8 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
       <c r="F55" s="17"/>
@@ -2171,8 +2221,8 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
@@ -2182,8 +2232,8 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
@@ -2193,8 +2243,8 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
@@ -2204,8 +2254,8 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
@@ -2215,8 +2265,8 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
       <c r="D60" s="17"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -2226,8 +2276,8 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
       <c r="D61" s="17"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
@@ -2237,41 +2287,259 @@
     </row>
   </sheetData>
   <mergeCells count="312">
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AA7:AC7"/>
+    <mergeCell ref="AA8:AC8"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="S39:T39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="S40:T40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O27:P27"/>
     <mergeCell ref="S28:T28"/>
     <mergeCell ref="S29:T29"/>
     <mergeCell ref="S30:T30"/>
@@ -2296,259 +2564,41 @@
     <mergeCell ref="O29:P29"/>
     <mergeCell ref="O30:P30"/>
     <mergeCell ref="O31:P31"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="S39:T39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="O40:P40"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="S40:T40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="O41:P41"/>
-    <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="O42:P42"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="S42:T42"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AA7:AC7"/>
-    <mergeCell ref="AA8:AC8"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>